<commit_message>
read regs from reg_map_module.xlsx
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="58">
   <si>
     <t>name</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>v_pwr</t>
+  </si>
+  <si>
+    <t>can</t>
   </si>
 </sst>
 </file>
@@ -300,6 +303,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -309,12 +318,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -616,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +631,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -639,16 +642,21 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -671,41 +679,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="2" max="2" width="21.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="12"/>
-    <col min="10" max="10" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="9"/>
+    <col min="10" max="10" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="9"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -764,46 +772,46 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="12"/>
-    <col min="10" max="10" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="9"/>
+    <col min="10" max="10" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="9"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -844,130 +852,130 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="7">
         <v>4</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="10">
-        <v>1</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>40</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="10">
-        <v>1</v>
-      </c>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="10">
-        <v>1</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="7">
         <v>12</v>
       </c>
     </row>
@@ -986,50 +994,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="2" max="2" width="21.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="12"/>
-    <col min="10" max="10" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="9"/>
+    <col min="10" max="10" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="9"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1070,101 +1078,101 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1192,41 +1200,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="12"/>
-    <col min="10" max="10" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="9"/>
+    <col min="10" max="10" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="9"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1267,78 +1275,78 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="7">
         <v>40</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1357,7 +1365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1366,41 +1374,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="10"/>
-    <col min="2" max="2" width="21.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="12"/>
-    <col min="10" max="10" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="9"/>
+    <col min="10" max="10" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="9"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1441,13 +1449,13 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reg validation in regs_handler.py
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="59">
   <si>
     <t>name</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>can</t>
+  </si>
+  <si>
+    <t>auto</t>
   </si>
 </sst>
 </file>
@@ -772,7 +775,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,6 +867,9 @@
       <c r="E3" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="F3" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -878,6 +884,9 @@
       <c r="E4" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="F4" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -889,6 +898,12 @@
       <c r="D5" s="7">
         <v>1</v>
       </c>
+      <c r="F5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -903,6 +918,9 @@
       <c r="E6" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="F6" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -914,6 +932,9 @@
       <c r="D7" s="7">
         <v>1</v>
       </c>
+      <c r="F7" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -925,6 +946,12 @@
       <c r="D8" s="7">
         <v>1</v>
       </c>
+      <c r="F8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -939,6 +966,9 @@
       <c r="E9" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="F9" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -953,6 +983,9 @@
       <c r="E10" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="F10" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -967,6 +1000,9 @@
       <c r="E11" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="F11" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -977,6 +1013,9 @@
       </c>
       <c r="D12" s="7">
         <v>12</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -994,11 +1033,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,6 +1126,9 @@
       <c r="D3" s="7">
         <v>1</v>
       </c>
+      <c r="F3" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1098,6 +1140,9 @@
       <c r="D4" s="7">
         <v>1</v>
       </c>
+      <c r="F4" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -1109,6 +1154,9 @@
       <c r="D5" s="7">
         <v>1</v>
       </c>
+      <c r="F5" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1120,6 +1168,9 @@
       <c r="D6" s="7">
         <v>1</v>
       </c>
+      <c r="F6" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1131,6 +1182,9 @@
       <c r="D7" s="7">
         <v>1</v>
       </c>
+      <c r="F7" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1142,6 +1196,9 @@
       <c r="D8" s="7">
         <v>1</v>
       </c>
+      <c r="F8" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -1153,6 +1210,9 @@
       <c r="D9" s="7">
         <v>1</v>
       </c>
+      <c r="F9" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1164,6 +1224,9 @@
       <c r="D10" s="7">
         <v>1</v>
       </c>
+      <c r="F10" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -1174,6 +1237,9 @@
       </c>
       <c r="D11" s="7">
         <v>1</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1195,7 +1261,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,6 +1353,9 @@
       <c r="E3" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="F3" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1301,6 +1370,9 @@
       <c r="E4" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="F4" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -1312,6 +1384,9 @@
       <c r="D5" s="7">
         <v>1</v>
       </c>
+      <c r="F5" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1323,6 +1398,12 @@
       <c r="D6" s="7">
         <v>1</v>
       </c>
+      <c r="F6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1334,20 +1415,35 @@
       <c r="D7" s="7">
         <v>40</v>
       </c>
+      <c r="F7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>54</v>
       </c>
+      <c r="F8" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>55</v>
       </c>
+      <c r="F9" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>56</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1365,11 +1461,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,6 +1554,12 @@
       <c r="D3" s="7">
         <v>1</v>
       </c>
+      <c r="F3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="10">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
MDBaddr and save_addr auto appointment bug fixed
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="60">
   <si>
     <t>name</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>auto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
   </si>
   <si>
     <t>serial_very_long_named_register_in _this_test_case</t>
@@ -777,7 +774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -924,8 +921,8 @@
       <c r="E6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="8">
-        <v>14</v>
+      <c r="F6" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="J6" s="10">
         <v>8</v>
@@ -978,8 +975,8 @@
       <c r="F9" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="10">
-        <v>22</v>
+      <c r="J9" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1015,8 +1012,8 @@
       <c r="F11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J11" s="10">
-        <v>14</v>
+      <c r="J11" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1029,8 +1026,8 @@
       <c r="D12" s="7">
         <v>12</v>
       </c>
-      <c r="F12" s="8">
-        <v>10</v>
+      <c r="F12" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1272,11 +1269,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,14 +1382,14 @@
       <c r="E4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="8">
-        <v>30</v>
+      <c r="F4" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>57</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1406,12 +1403,12 @@
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>33</v>
@@ -1436,8 +1433,8 @@
       <c r="D7" s="7">
         <v>40</v>
       </c>
-      <c r="F7" s="8">
-        <v>50</v>
+      <c r="F7" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
clear main.c/h for build
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -789,11 +789,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,7 +1076,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,11 +1296,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
generator - removed time struct
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>s8</t>
-  </si>
-  <si>
-    <t>time</t>
   </si>
   <si>
     <t>runtime</t>
@@ -640,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,21 +660,16 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -877,7 +869,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>29</v>
@@ -889,7 +881,7 @@
         <v>28</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -897,7 +889,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>30</v>
@@ -909,7 +901,7 @@
         <v>28</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -917,7 +909,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>29</v>
@@ -926,10 +918,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -937,10 +929,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="7">
         <v>40</v>
@@ -949,7 +941,7 @@
         <v>28</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J6" s="10">
         <v>8</v>
@@ -966,12 +958,12 @@
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>30</v>
@@ -980,15 +972,15 @@
         <v>1</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>32</v>
@@ -1000,15 +992,15 @@
         <v>28</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>32</v>
@@ -1020,15 +1012,15 @@
         <v>28</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
@@ -1037,15 +1029,15 @@
         <v>28</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>29</v>
@@ -1054,7 +1046,7 @@
         <v>12</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1166,7 +1158,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1180,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1194,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1208,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1222,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1236,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1250,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1264,7 +1256,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1278,7 +1270,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1296,7 +1288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1393,7 +1385,7 @@
         <v>28</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1401,7 +1393,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="7">
         <v>40</v>
@@ -1410,13 +1402,13 @@
         <v>28</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1430,12 +1422,12 @@
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>32</v>
@@ -1444,10 +1436,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1455,49 +1447,49 @@
         <v>25</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="7">
         <v>40</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1603,7 +1595,7 @@
         <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>29</v>
@@ -1612,7 +1604,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J3" s="10">
         <v>4</v>

</xml_diff>

<commit_message>
added test arrays for modbus
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9DF8F3-2C6F-40A3-92A1-664114DB9479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455FF81C-82AB-4219-9834-BE0FD68BC332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="device" sheetId="5" r:id="rId5"/>
     <sheet name="modbus" sheetId="7" r:id="rId6"/>
     <sheet name="service" sheetId="9" r:id="rId7"/>
+    <sheet name="test" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="113">
   <si>
     <t>name</t>
   </si>
@@ -326,6 +327,57 @@
   </si>
   <si>
     <t>rs485_state</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>arr_u8</t>
+  </si>
+  <si>
+    <t>arr_u16</t>
+  </si>
+  <si>
+    <t>arr_u32</t>
+  </si>
+  <si>
+    <t>arr_u64</t>
+  </si>
+  <si>
+    <t>arr_s8</t>
+  </si>
+  <si>
+    <t>arr_s16</t>
+  </si>
+  <si>
+    <t>arr_s32</t>
+  </si>
+  <si>
+    <t>arr_s64</t>
+  </si>
+  <si>
+    <t>arr_float</t>
+  </si>
+  <si>
+    <t>arr_char</t>
+  </si>
+  <si>
+    <t>u64</t>
+  </si>
+  <si>
+    <t>s16</t>
+  </si>
+  <si>
+    <t>s32</t>
+  </si>
+  <si>
+    <t>s64</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>arr_double</t>
   </si>
 </sst>
 </file>
@@ -762,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,6 +853,11 @@
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -915,7 +972,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1824,7 +1881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F146BD-F89E-4E15-A02E-16005116AC05}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1984,4 +2041,256 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FF13CE-6448-41FA-BA7B-6B713DD2EE28}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="9"/>
+    <col min="10" max="10" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="7">
+        <v>20</v>
+      </c>
+      <c r="F3" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="7">
+        <v>20</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="7">
+        <v>20</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="7">
+        <v>20</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="7">
+        <v>20</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="7">
+        <v>20</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="7">
+        <v>20</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="7">
+        <v>20</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="7">
+        <v>20</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="7">
+        <v>20</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="7">
+        <v>20</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add device info into regs
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455FF81C-82AB-4219-9834-BE0FD68BC332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D70B2E-4A75-43C7-9EF4-90288466D855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="114">
   <si>
     <t>name</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>auto</t>
-  </si>
-  <si>
-    <t>User</t>
   </si>
   <si>
     <t>char</t>
@@ -378,6 +375,12 @@
   </si>
   <si>
     <t>arr_double</t>
+  </si>
+  <si>
+    <t>build_date</t>
+  </si>
+  <si>
+    <t>Date of SW building</t>
   </si>
 </sst>
 </file>
@@ -837,7 +840,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -852,12 +855,12 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -966,13 +969,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q14" sqref="Q14"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,10 +1059,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="7">
         <v>4</v>
@@ -1076,7 +1079,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>30</v>
@@ -1096,10 +1099,10 @@
         <v>24</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
@@ -1116,10 +1119,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="7">
         <v>40</v>
@@ -1130,22 +1133,22 @@
       <c r="F6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J6" s="10">
-        <v>8</v>
-      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D7" s="7">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>54</v>
@@ -1153,10 +1156,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>30</v>
@@ -1167,25 +1170,19 @@
       <c r="F8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="10" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>54</v>
@@ -1196,7 +1193,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>73</v>
@@ -1213,16 +1210,19 @@
       <c r="F10" s="8" t="s">
         <v>54</v>
       </c>
+      <c r="J10" s="10" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
@@ -1233,24 +1233,47 @@
       <c r="F11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="10" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7">
         <v>12</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="E13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1273,7 +1296,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,7 +1380,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>30</v>
@@ -1374,10 +1397,10 @@
         <v>36</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
@@ -1391,10 +1414,10 @@
         <v>37</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
@@ -1408,10 +1431,10 @@
         <v>38</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
@@ -1425,10 +1448,10 @@
         <v>39</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
@@ -1442,10 +1465,10 @@
         <v>40</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
@@ -1459,7 +1482,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>30</v>
@@ -1476,7 +1499,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>32</v>
@@ -1493,10 +1516,10 @@
         <v>43</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
@@ -1520,11 +1543,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,10 +1631,10 @@
         <v>21</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
@@ -1628,10 +1651,10 @@
         <v>26</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="7">
         <v>40</v>
@@ -1644,9 +1667,6 @@
       </c>
       <c r="J4" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1654,10 +1674,10 @@
         <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
@@ -1668,10 +1688,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>32</v>
@@ -1691,10 +1711,10 @@
         <v>25</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="7">
         <v>40</v>
@@ -1711,10 +1731,13 @@
         <v>51</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>49</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>54</v>
@@ -1725,10 +1748,13 @@
         <v>52</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>49</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>54</v>
@@ -1739,10 +1765,13 @@
         <v>53</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>49</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>54</v>
@@ -1767,7 +1796,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1851,10 +1880,10 @@
         <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
@@ -1966,10 +1995,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>32</v>
@@ -1983,10 +2012,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>32</v>
@@ -2000,10 +2029,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>32</v>
@@ -2017,10 +2046,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>32</v>
@@ -2047,7 +2076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FF13CE-6448-41FA-BA7B-6B713DD2EE28}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -2132,7 +2161,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>29</v>
@@ -2146,7 +2175,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>30</v>
@@ -2160,7 +2189,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>32</v>
@@ -2174,10 +2203,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="7">
         <v>20</v>
@@ -2188,7 +2217,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>44</v>
@@ -2202,10 +2231,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8" s="7">
         <v>20</v>
@@ -2216,10 +2245,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="7">
         <v>20</v>
@@ -2230,10 +2259,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="7">
         <v>20</v>
@@ -2244,7 +2273,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>49</v>
@@ -2258,10 +2287,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" s="7">
         <v>20</v>
@@ -2272,10 +2301,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="7">
         <v>20</v>

</xml_diff>

<commit_message>
Service channels measuring by Internal ADC released
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D70B2E-4A75-43C7-9EF4-90288466D855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B5F58E-75D8-4B8A-846A-2972A27673A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="118">
   <si>
     <t>name</t>
   </si>
@@ -381,6 +381,18 @@
   </si>
   <si>
     <t>Date of SW building</t>
+  </si>
+  <si>
+    <t>vref_int</t>
+  </si>
+  <si>
+    <t>vref_ext</t>
+  </si>
+  <si>
+    <t>Vref internal (V)</t>
+  </si>
+  <si>
+    <t>Vref external (V)</t>
   </si>
 </sst>
 </file>
@@ -1541,13 +1553,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,7 +1570,8 @@
     <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="9"/>
+    <col min="7" max="7" width="10.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="9"/>
     <col min="10" max="10" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
@@ -1774,6 +1787,40 @@
         <v>28</v>
       </c>
       <c r="F10" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ai regs added to regs_map corrected
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B5F58E-75D8-4B8A-846A-2972A27673A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C023F73-D06F-4C11-9474-24498246C495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -20,14 +20,15 @@
     <sheet name="device" sheetId="5" r:id="rId5"/>
     <sheet name="modbus" sheetId="7" r:id="rId6"/>
     <sheet name="service" sheetId="9" r:id="rId7"/>
-    <sheet name="test" sheetId="10" r:id="rId8"/>
+    <sheet name="ai" sheetId="11" r:id="rId8"/>
+    <sheet name="test" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="128">
   <si>
     <t>name</t>
   </si>
@@ -302,15 +303,9 @@
     <t>rtc_state</t>
   </si>
   <si>
-    <t>adc_state</t>
-  </si>
-  <si>
     <t>RTC service status</t>
   </si>
   <si>
-    <t>ADC service status</t>
-  </si>
-  <si>
     <t>service</t>
   </si>
   <si>
@@ -320,9 +315,6 @@
     <t>dbg_state</t>
   </si>
   <si>
-    <t>RS485 service status</t>
-  </si>
-  <si>
     <t>rs485_state</t>
   </si>
   <si>
@@ -393,6 +385,45 @@
   </si>
   <si>
     <t>Vref external (V)</t>
+  </si>
+  <si>
+    <t>ai_value</t>
+  </si>
+  <si>
+    <t>ai_calib_a</t>
+  </si>
+  <si>
+    <t>ai_calib_b</t>
+  </si>
+  <si>
+    <t>ai_adc</t>
+  </si>
+  <si>
+    <t>ai_sample_rate</t>
+  </si>
+  <si>
+    <t>Measured value</t>
+  </si>
+  <si>
+    <t>Calibration coef A</t>
+  </si>
+  <si>
+    <t>Calibration coef B</t>
+  </si>
+  <si>
+    <t>ADC raw data</t>
+  </si>
+  <si>
+    <t>adc_int_state</t>
+  </si>
+  <si>
+    <t>ADC_INT service status</t>
+  </si>
+  <si>
+    <t>RS-485 service status</t>
+  </si>
+  <si>
+    <t>Samples per second</t>
   </si>
 </sst>
 </file>
@@ -867,12 +898,12 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -993,7 +1024,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -1148,10 +1179,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>55</v>
@@ -1531,7 +1562,7 @@
         <v>85</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
@@ -1555,11 +1586,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,10 +1823,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>49</v>
@@ -1809,10 +1840,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>49</v>
@@ -1849,7 +1880,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="7" customWidth="1"/>
     <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -1961,12 +1992,12 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
@@ -2045,7 +2076,7 @@
         <v>86</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>32</v>
@@ -2059,10 +2090,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>32</v>
@@ -2076,10 +2107,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>32</v>
@@ -2093,10 +2124,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>32</v>
@@ -2120,6 +2151,204 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622EF646-023E-42FD-8335-9337B02D684D}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="9"/>
+    <col min="10" max="10" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FF13CE-6448-41FA-BA7B-6B713DD2EE28}">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -2208,7 +2437,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>29</v>
@@ -2222,7 +2451,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>30</v>
@@ -2236,7 +2465,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>32</v>
@@ -2250,10 +2479,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D6" s="7">
         <v>20</v>
@@ -2264,7 +2493,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>44</v>
@@ -2278,10 +2507,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D8" s="7">
         <v>20</v>
@@ -2292,10 +2521,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D9" s="7">
         <v>20</v>
@@ -2306,10 +2535,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D10" s="7">
         <v>20</v>
@@ -2320,7 +2549,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>49</v>
@@ -2334,10 +2563,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D12" s="7">
         <v>20</v>
@@ -2348,7 +2577,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
AI channels measure released
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C023F73-D06F-4C11-9474-24498246C495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52459F6E-271E-4AFA-A7D7-069265C6029A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -20,15 +20,16 @@
     <sheet name="device" sheetId="5" r:id="rId5"/>
     <sheet name="modbus" sheetId="7" r:id="rId6"/>
     <sheet name="service" sheetId="9" r:id="rId7"/>
-    <sheet name="ai" sheetId="11" r:id="rId8"/>
-    <sheet name="test" sheetId="10" r:id="rId9"/>
+    <sheet name="debug" sheetId="12" r:id="rId8"/>
+    <sheet name="ai" sheetId="11" r:id="rId9"/>
+    <sheet name="test" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="132">
   <si>
     <t>name</t>
   </si>
@@ -424,6 +425,18 @@
   </si>
   <si>
     <t>Samples per second</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>ai_state</t>
+  </si>
+  <si>
+    <t>AI service status</t>
+  </si>
+  <si>
+    <t>debug</t>
   </si>
 </sst>
 </file>
@@ -860,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,10 +916,272 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FF13CE-6448-41FA-BA7B-6B713DD2EE28}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="9"/>
+    <col min="10" max="10" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="7">
+        <v>20</v>
+      </c>
+      <c r="F3" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="7">
+        <v>20</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="7">
+        <v>20</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="7">
+        <v>20</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="7">
+        <v>20</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="7">
+        <v>20</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="7">
+        <v>20</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="7">
+        <v>20</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="7">
+        <v>20</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="7">
+        <v>20</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="7">
+        <v>20</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1986,13 +2261,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F146BD-F89E-4E15-A02E-16005116AC05}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2139,6 +2414,23 @@
         <v>54</v>
       </c>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
@@ -2151,14 +2443,112 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4ADAE7-8217-4070-BB60-AD1572F84295}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="9"/>
+    <col min="10" max="10" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622EF646-023E-42FD-8335-9337B02D684D}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,8 +2643,8 @@
       <c r="E3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>54</v>
+      <c r="F3" s="8">
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2270,8 +2660,8 @@
       <c r="D4" s="7">
         <v>2</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>54</v>
+      <c r="F4" s="8">
+        <v>204</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>54</v>
@@ -2290,8 +2680,8 @@
       <c r="D5" s="7">
         <v>2</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>54</v>
+      <c r="F5" s="8">
+        <v>208</v>
       </c>
       <c r="J5" s="10" t="s">
         <v>54</v>
@@ -2313,8 +2703,8 @@
       <c r="E6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>54</v>
+      <c r="F6" s="8">
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2333,260 +2723,8 @@
       <c r="E7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="K1:L1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FF13CE-6448-41FA-BA7B-6B713DD2EE28}">
-  <dimension ref="A1:L13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="9"/>
-    <col min="10" max="10" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="15"/>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="7">
-        <v>20</v>
-      </c>
-      <c r="F3" s="8">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="7">
-        <v>20</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="7">
-        <v>20</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="7">
-        <v>20</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="7">
-        <v>20</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="7">
-        <v>20</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" s="7">
-        <v>20</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="7">
-        <v>20</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="7">
-        <v>20</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="7">
-        <v>20</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="7">
-        <v>20</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>54</v>
+      <c r="F7" s="8">
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed all SOFI to SAND
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BB380D-5542-4AA3-A0B2-546C8867DC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD329FB0-0554-40E6-BB91-DC82F9BFB369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -43,18 +43,9 @@
     <t>read_only</t>
   </si>
   <si>
-    <t>SOFI_PROP_BASE</t>
-  </si>
-  <si>
     <t>mdb_addr</t>
   </si>
   <si>
-    <t>SOFI_PROP_MDB</t>
-  </si>
-  <si>
-    <t>SOFI_PROP_RANGE</t>
-  </si>
-  <si>
     <t>p_def</t>
   </si>
   <si>
@@ -65,12 +56,6 @@
   </si>
   <si>
     <t>save_addr</t>
-  </si>
-  <si>
-    <t>SOFI_PROP_SAVE</t>
-  </si>
-  <si>
-    <t>SOFI_PROP_ACCESS</t>
   </si>
   <si>
     <t>access_lvl</t>
@@ -449,6 +434,21 @@
   </si>
   <si>
     <t>Unique MCU ID number</t>
+  </si>
+  <si>
+    <t>SAND_PROP_BASE</t>
+  </si>
+  <si>
+    <t>SAND_PROP_MDB</t>
+  </si>
+  <si>
+    <t>SAND_PROP_RANGE</t>
+  </si>
+  <si>
+    <t>SAND_PROP_SAVE</t>
+  </si>
+  <si>
+    <t>SAND_PROP_ACCESS</t>
   </si>
 </sst>
 </file>
@@ -898,47 +898,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -951,11 +951,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FF13CE-6448-41FA-BA7B-6B713DD2EE28}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,25 +974,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -1001,7 +1001,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
@@ -1013,179 +1013,179 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D3" s="7">
         <v>20</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="7">
         <v>20</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D5" s="7">
         <v>20</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D6" s="7">
         <v>20</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D7" s="7">
         <v>20</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D8" s="7">
         <v>20</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D9" s="7">
         <v>20</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D10" s="7">
         <v>20</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D11" s="7">
         <v>20</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D12" s="7">
         <v>20</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D13" s="7">
         <v>20</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1203,7 +1203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1226,25 +1226,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -1253,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
@@ -1265,25 +1265,25 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1324,25 +1324,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -1351,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
@@ -1363,228 +1363,228 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D3" s="7">
         <v>4</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="7">
-        <v>1</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D6" s="7">
         <v>40</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D7" s="7">
         <v>40</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1625,25 +1625,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -1652,7 +1652,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
@@ -1664,178 +1664,178 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1857,7 +1857,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,25 +1877,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
@@ -1916,270 +1916,270 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D3" s="7">
         <v>40</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D4" s="7">
         <v>40</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D5" s="7">
         <v>40</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D6" s="7">
         <v>40</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D7" s="7">
         <v>12</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2220,25 +2220,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -2247,7 +2247,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
@@ -2259,42 +2259,42 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J3" s="10">
         <v>4</v>
@@ -2338,25 +2338,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -2365,7 +2365,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
@@ -2377,110 +2377,110 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E3" s="7">
         <v>1</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E5" s="7">
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E6" s="7">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2521,25 +2521,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -2548,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
@@ -2560,25 +2560,25 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2600,7 +2600,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4:F7"/>
+      <selection pane="bottomRight" activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,25 +2619,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>13</v>
+        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -2646,7 +2646,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
@@ -2658,125 +2658,125 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>117</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7">
         <v>2</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>118</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D4" s="7">
         <v>2</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>119</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D5" s="7">
         <v>2</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>120</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D6" s="7">
         <v>2</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D7" s="7">
         <v>2</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generator: regs names added
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD329FB0-0554-40E6-BB91-DC82F9BFB369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2CBB9C-A6BA-4435-910F-9285E3E286EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="135">
   <si>
     <t>name</t>
   </si>
@@ -410,9 +410,6 @@
   </si>
   <si>
     <t>AI service status</t>
-  </si>
-  <si>
-    <t>debug</t>
   </si>
   <si>
     <t>MCU information</t>
@@ -885,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,16 +925,11 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
         <v>84</v>
       </c>
     </row>
@@ -951,7 +943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FF13CE-6448-41FA-BA7B-6B713DD2EE28}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -974,25 +966,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -1226,25 +1218,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -1324,25 +1316,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -1409,7 +1401,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>25</v>
@@ -1625,25 +1617,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -1857,7 +1849,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q17" sqref="Q17"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,25 +1869,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -1959,10 +1951,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>49</v>
@@ -1999,10 +1991,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>49</v>
@@ -2019,10 +2011,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>24</v>
@@ -2220,25 +2212,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -2338,25 +2330,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -2502,7 +2494,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,25 +2513,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>
@@ -2619,25 +2611,25 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>133</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="L1" s="15"/>
     </row>

</xml_diff>

<commit_message>
generator: step desription added in error message
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2CBB9C-A6BA-4435-910F-9285E3E286EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D7D837-FD84-40AB-BD25-E8AE33D0EC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -884,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -1293,7 +1293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1467,7 +1467,7 @@
         <v>49</v>
       </c>
       <c r="D7" s="7">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>23</v>
@@ -1849,7 +1849,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
generator: const range list added
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D7D837-FD84-40AB-BD25-E8AE33D0EC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D761EAF1-B28B-4D05-B00B-DF33751A8C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="141">
   <si>
     <t>name</t>
   </si>
@@ -446,6 +446,24 @@
   </si>
   <si>
     <t>SAND_PROP_ACCESS</t>
+  </si>
+  <si>
+    <t>{17,0,4,2,5}</t>
+  </si>
+  <si>
+    <t>"Hello world!"</t>
+  </si>
+  <si>
+    <t>{15.4f, 71.524f}</t>
+  </si>
+  <si>
+    <t>-12.5f</t>
+  </si>
+  <si>
+    <t>255.44f</t>
+  </si>
+  <si>
+    <t>{15.4f,71.524f}</t>
   </si>
 </sst>
 </file>
@@ -543,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -578,6 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -943,11 +962,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FF13CE-6448-41FA-BA7B-6B713DD2EE28}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O15" sqref="O15"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +977,8 @@
     <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="9"/>
+    <col min="7" max="7" width="16.140625" style="9" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="9"/>
     <col min="10" max="10" width="16.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
@@ -1039,6 +1059,9 @@
       <c r="F3" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="G3" s="9" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1151,6 +1174,15 @@
       <c r="F11" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="G11" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -1165,6 +1197,9 @@
       <c r="F12" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="G12" s="9" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1178,6 +1213,9 @@
       </c>
       <c r="F13" s="8" t="s">
         <v>48</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1293,7 +1331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1598,7 +1636,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,6 +1748,12 @@
       <c r="F4" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -1727,6 +1771,12 @@
       <c r="F5" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1744,6 +1794,12 @@
       <c r="F6" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="H6" s="9">
+        <v>0</v>
+      </c>
+      <c r="I6" s="9">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1761,6 +1817,12 @@
       <c r="F7" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="H7" s="9">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1778,6 +1840,12 @@
       <c r="F8" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>59</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -1795,6 +1863,12 @@
       <c r="F9" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="H9" s="9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9">
+        <v>999</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1828,6 +1902,12 @@
       </c>
       <c r="F11" s="8" t="s">
         <v>48</v>
+      </c>
+      <c r="H11" s="9">
+        <v>-12</v>
+      </c>
+      <c r="I11" s="9">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generagor messages are colored
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5421FDD5-4776-4822-8431-590FAD863625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263E0BCA-CE16-4197-ABC4-DA0220B97668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="137">
   <si>
     <t>name</t>
   </si>
@@ -575,6 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -584,7 +585,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -950,11 +950,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FF13CE-6448-41FA-BA7B-6B713DD2EE28}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3:I13"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,28 +973,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="15"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1159,7 +1159,7 @@
       <c r="F11" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="16"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -1183,7 +1183,7 @@
         <v>49</v>
       </c>
       <c r="D13" s="7">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>48</v>
@@ -1226,28 +1226,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="15"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1306,7 +1306,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,28 +1324,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="15"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1582,9 +1582,6 @@
         <v>23</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1607,7 +1604,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,28 +1622,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="15"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1919,28 +1916,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="15"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2262,28 +2259,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="15"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2380,28 +2377,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="15"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2563,28 +2560,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="15"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2639,7 +2636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622EF646-023E-42FD-8335-9337B02D684D}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -2662,28 +2659,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="L1" s="15"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">

</xml_diff>

<commit_message>
dump verification test (not done)
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967B3FF3-503B-4285-97CA-7295E4337353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEB258F-0B1C-432A-997F-7E38367757B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="172">
   <si>
     <t>name</t>
   </si>
@@ -1064,7 +1064,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,11 +1478,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,7 +1786,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="A9:E10"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,9 +1905,6 @@
       <c r="F4" s="8">
         <v>240</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -1928,9 +1925,6 @@
       <c r="F5" s="8">
         <v>280</v>
       </c>
-      <c r="J5" s="10" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -2011,9 +2005,6 @@
       <c r="F9" s="8">
         <v>367</v>
       </c>
-      <c r="J9" s="10" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -2033,9 +2024,6 @@
       </c>
       <c r="F10" s="8">
         <v>368</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2675,7 +2663,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4:E5"/>
+      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2937,7 +2925,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3038,9 +3026,6 @@
       <c r="I3" s="9">
         <v>255</v>
       </c>
-      <c r="J3" s="10" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -3063,9 +3048,6 @@
       </c>
       <c r="I4" s="9">
         <v>1</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3143,11 +3125,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622EF646-023E-42FD-8335-9337B02D684D}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3269,9 +3251,6 @@
       <c r="G4" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -3294,9 +3273,6 @@
       </c>
       <c r="G5" s="9" t="s">
         <v>134</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
os calobration regs added
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73647627-D326-47F0-B36A-29612E42E5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063407A7-7B68-47D4-A011-40509C38B814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="180">
   <si>
     <t>name</t>
   </si>
@@ -557,6 +557,30 @@
   </si>
   <si>
     <t>Error packet counter</t>
+  </si>
+  <si>
+    <t>tmpr_add</t>
+  </si>
+  <si>
+    <t>v_pwr_mul</t>
+  </si>
+  <si>
+    <t>vref_sel</t>
+  </si>
+  <si>
+    <t>0.0f</t>
+  </si>
+  <si>
+    <t>16.0f</t>
+  </si>
+  <si>
+    <t>Power voltage calibration multiple coefficient</t>
+  </si>
+  <si>
+    <t>Temperature calibration additional coefficient</t>
+  </si>
+  <si>
+    <t>Select Vref source (0-Vref_int, 1-Vref_ext)</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FF13CE-6448-41FA-BA7B-6B713DD2EE28}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1482,7 +1506,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,6 +1644,15 @@
       <c r="F5" s="8">
         <v>5</v>
       </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1</v>
+      </c>
       <c r="J5" s="10" t="s">
         <v>48</v>
       </c>
@@ -1783,19 +1816,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -1923,7 +1956,7 @@
         <v>49</v>
       </c>
       <c r="D5" s="7">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>152</v>
@@ -2139,6 +2172,90 @@
       </c>
       <c r="F15" s="8">
         <v>378</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16" s="8">
+        <v>380</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="8">
+        <v>382</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18" s="8">
+        <v>384</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0</v>
+      </c>
+      <c r="H18" s="9">
+        <v>0</v>
+      </c>
+      <c r="I18" s="9">
+        <v>1</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vpwr caltulate by calibration coefs
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063407A7-7B68-47D4-A011-40509C38B814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3109CF-24E4-4C3A-B766-F6D3A9C2D04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="182">
   <si>
     <t>name</t>
   </si>
@@ -581,6 +581,12 @@
   </si>
   <si>
     <t>Select Vref source (0-Vref_int, 1-Vref_ext)</t>
+  </si>
+  <si>
+    <t>v_pwr_add</t>
+  </si>
+  <si>
+    <t>Power voltage calibration additional coefficient</t>
   </si>
 </sst>
 </file>
@@ -1816,19 +1822,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -2228,13 +2234,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D18" s="7">
         <v>1</v>
@@ -2245,16 +2251,42 @@
       <c r="F18" s="8">
         <v>384</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" s="8">
+        <v>386</v>
+      </c>
+      <c r="G19" s="9">
         <v>0</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H19" s="9">
         <v>0</v>
       </c>
-      <c r="I18" s="9">
-        <v>1</v>
-      </c>
-      <c r="J18" s="10" t="s">
+      <c r="I19" s="9">
+        <v>1</v>
+      </c>
+      <c r="J19" s="10" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
storage regs modified into regs_map
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335FFDB0-A4A9-4CA4-91D2-0F81B996C91F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387BF6D6-A82B-4284-8580-6CAF34764C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="186">
   <si>
     <t>name</t>
   </si>
@@ -587,6 +587,18 @@
   </si>
   <si>
     <t>Power voltage calibration additional coefficient</t>
+  </si>
+  <si>
+    <t>dump_position</t>
+  </si>
+  <si>
+    <t>storage_size</t>
+  </si>
+  <si>
+    <t>Storage FLASH size (bytes)</t>
+  </si>
+  <si>
+    <t>Save dump FLASH position</t>
   </si>
 </sst>
 </file>
@@ -1512,7 +1524,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,13 +2830,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4ADAE7-8217-4070-BB60-AD1572F84295}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3029,10 +3041,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>142</v>
+        <v>182</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>148</v>
+        <v>185</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>25</v>
@@ -3049,10 +3061,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>25</v>
@@ -3065,6 +3077,46 @@
       </c>
       <c r="F9" s="8">
         <v>609</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="8">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="8">
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -3082,7 +3134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>

<commit_message>
Set RDP for RELEASE
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387BF6D6-A82B-4284-8580-6CAF34764C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FC5E7C-077F-41E8-8D51-4DB3103ED034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="190">
   <si>
     <t>name</t>
   </si>
@@ -599,6 +599,18 @@
   </si>
   <si>
     <t>Save dump FLASH position</t>
+  </si>
+  <si>
+    <t>reset_reason</t>
+  </si>
+  <si>
+    <t>Reason of last reset</t>
+  </si>
+  <si>
+    <t>release</t>
+  </si>
+  <si>
+    <t>Release flag</t>
   </si>
 </sst>
 </file>
@@ -1518,13 +1530,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,13 +1732,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>40</v>
+        <v>186</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
@@ -1740,13 +1752,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>41</v>
+        <v>188</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>65</v>
+        <v>189</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
@@ -1755,18 +1767,18 @@
         <v>23</v>
       </c>
       <c r="F9" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
@@ -1775,46 +1787,86 @@
         <v>23</v>
       </c>
       <c r="F10" s="8">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D11" s="7">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="8">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D12" s="7">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="7">
+        <v>40</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="7">
+        <v>20</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="8">
         <v>60</v>
       </c>
     </row>
@@ -1834,7 +1886,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
@@ -2832,7 +2884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4ADAE7-8217-4070-BB60-AD1572F84295}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3138,7 +3190,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
release flag added to regs_map
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387BF6D6-A82B-4284-8580-6CAF34764C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FC5E7C-077F-41E8-8D51-4DB3103ED034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="190">
   <si>
     <t>name</t>
   </si>
@@ -599,6 +599,18 @@
   </si>
   <si>
     <t>Save dump FLASH position</t>
+  </si>
+  <si>
+    <t>reset_reason</t>
+  </si>
+  <si>
+    <t>Reason of last reset</t>
+  </si>
+  <si>
+    <t>release</t>
+  </si>
+  <si>
+    <t>Release flag</t>
   </si>
 </sst>
 </file>
@@ -1518,13 +1530,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1720,13 +1732,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>40</v>
+        <v>186</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>66</v>
+        <v>187</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
@@ -1740,13 +1752,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>41</v>
+        <v>188</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>65</v>
+        <v>189</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
@@ -1755,18 +1767,18 @@
         <v>23</v>
       </c>
       <c r="F9" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
@@ -1775,46 +1787,86 @@
         <v>23</v>
       </c>
       <c r="F10" s="8">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D11" s="7">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="8">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>101</v>
+        <v>43</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D12" s="7">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="7">
+        <v>40</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="7">
+        <v>20</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="8">
         <v>60</v>
       </c>
     </row>
@@ -1834,7 +1886,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
@@ -2832,7 +2884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4ADAE7-8217-4070-BB60-AD1572F84295}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3138,7 +3190,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Save data to storage during shutdown
</commit_message>
<xml_diff>
--- a/generator/input/reg_maps/reg_map_sand_ai.xlsx
+++ b/generator/input/reg_maps/reg_map_sand_ai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Hobby\SAND\generator\input\reg_maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FC5E7C-077F-41E8-8D51-4DB3103ED034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F49BD8-4F40-4D2D-969E-360B39E9AC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="struct_list" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="194">
   <si>
     <t>name</t>
   </si>
@@ -611,6 +611,18 @@
   </si>
   <si>
     <t>Release flag</t>
+  </si>
+  <si>
+    <t>runtime_storage</t>
+  </si>
+  <si>
+    <t>Runtime before last reset (sec)</t>
+  </si>
+  <si>
+    <t>duration_us</t>
+  </si>
+  <si>
+    <t>Duration of save operation (us)</t>
   </si>
 </sst>
 </file>
@@ -1530,19 +1542,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -1792,10 +1804,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>41</v>
+        <v>190</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>27</v>
@@ -1809,16 +1821,19 @@
       <c r="F11" s="8">
         <v>12</v>
       </c>
+      <c r="J11" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
@@ -1832,41 +1847,61 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D13" s="7">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F13" s="8">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>49</v>
       </c>
       <c r="D14" s="7">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="7">
+        <v>20</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="8">
         <v>60</v>
       </c>
     </row>
@@ -2882,19 +2917,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4ADAE7-8217-4070-BB60-AD1572F84295}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" style="7" customWidth="1"/>
     <col min="3" max="3" width="5" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
@@ -3169,6 +3204,26 @@
       </c>
       <c r="F11" s="8">
         <v>611</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="8">
+        <v>612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>